<commit_message>
pause start functionality flask
</commit_message>
<xml_diff>
--- a/app/COVID19master/data/policy_example.xlsx
+++ b/app/COVID19master/data/policy_example.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chaitra Gopalappa\Documents\Box Sync\Paper\COVID-19\COVID19-master\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eleanor/Documents/GitHub/COVID19/Web/pre_run/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A79E63C-F3E7-004C-942C-3EDCD9B1025E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11100"/>
+    <workbookView xWindow="9080" yWindow="700" windowWidth="27900" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Decision" sheetId="1" r:id="rId1"/>
-    <sheet name="Unit Cost" sheetId="2" r:id="rId2"/>
+    <sheet name="Template" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>Start day</t>
   </si>
@@ -36,7 +37,16 @@
     <t xml:space="preserve">Cost per test </t>
   </si>
   <si>
+    <t>Contact tracing and testing</t>
+  </si>
+  <si>
+    <t>Universal testing</t>
+  </si>
+  <si>
     <t>Source</t>
+  </si>
+  <si>
+    <t>https://www.cms.gov/files/document/mac-covid-19-test-pricing.pdf</t>
   </si>
   <si>
     <t>Value (US$)</t>
@@ -51,6 +61,12 @@
     <t>0.5 upto day 30 --&gt;</t>
   </si>
   <si>
+    <t>10 upto day 12 --&gt;</t>
+  </si>
+  <si>
+    <t>100 upto day 27 --&gt;</t>
+  </si>
+  <si>
     <t>Simulate until day 100--&gt;</t>
   </si>
   <si>
@@ -63,50 +79,29 @@
     <t>1. Enter as many options as needed in each row</t>
   </si>
   <si>
+    <t>2. Last day wil be used as  run time of simulation, you can enter any number but keep it consistent across all three decisions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of testings per day through contact tracing </t>
+  </si>
+  <si>
+    <t>Number of testings per day through universal testing</t>
+  </si>
+  <si>
     <t>Propotion contact reduction (0 to 1)</t>
   </si>
   <si>
-    <t xml:space="preserve">Testing capacity per day through contact tracing </t>
+    <t>Testings per day</t>
   </si>
   <si>
-    <t>Median wage for unemployment (per day)</t>
-  </si>
-  <si>
-    <t>Contact tracing and testing (per person)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Universal testing (per person) </t>
-  </si>
-  <si>
-    <t>"How many workers are employed in sectors directly affected by COVID-19 shutdowns, where do they work, and how much do they earn?" United States Bureau of Labor Statistics, https://www.bls.gov/opub/mlr/2020/article/covid-19-shutdowns.htm</t>
-  </si>
-  <si>
-    <t>"Medicare Administrative Contractor (MAC) COVID-19 Test Pricing." Centers for Medicare&amp; Medicaid Services, https://www.cms.gov/files/document/mac-covid-19-test-pricing.pdf</t>
-  </si>
-  <si>
-    <t>Testing capacity per day through universal testing</t>
-  </si>
-  <si>
-    <t>Tests per day</t>
-  </si>
-  <si>
-    <t>100 tests upto day 27 --&gt;</t>
-  </si>
-  <si>
-    <t>300 tests upto day 100 --&gt;</t>
-  </si>
-  <si>
-    <t>10 tests upto day 12    --&gt;</t>
-  </si>
-  <si>
-    <t>2. Day on last row wil be used as run time of simulation, you can enter any number but keep it consistent across all three decisions</t>
+    <t xml:space="preserve">2. See plots to verify timeline of decision that will be modeled </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -141,20 +136,6 @@
       <b/>
       <sz val="12"/>
       <color theme="9" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -303,11 +284,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -349,29 +329,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -682,80 +654,77 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J390"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I390"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.875" style="12" customWidth="1"/>
-    <col min="3" max="3" width="18.125" style="9" customWidth="1"/>
-    <col min="4" max="4" width="18.875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.875" style="12" customWidth="1"/>
-    <col min="6" max="6" width="18.125" style="9" customWidth="1"/>
-    <col min="7" max="7" width="19.625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="18.875" style="12" customWidth="1"/>
-    <col min="9" max="9" width="18.125" style="9" customWidth="1"/>
-    <col min="10" max="10" width="58.5" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="10.875" style="1"/>
+    <col min="1" max="1" width="23.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.83203125" style="12" customWidth="1"/>
+    <col min="3" max="3" width="18.1640625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="18.83203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.83203125" style="12" customWidth="1"/>
+    <col min="6" max="6" width="18.1640625" style="9" customWidth="1"/>
+    <col min="7" max="7" width="19.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="18.83203125" style="12" customWidth="1"/>
+    <col min="9" max="9" width="18.1640625" style="9" customWidth="1"/>
+    <col min="10" max="10" width="10.1640625" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="2" customFormat="1" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="21"/>
-      <c r="E1" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="21"/>
-      <c r="H1" s="20" t="s">
+      <c r="B1" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="18"/>
+      <c r="E1" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="18"/>
+      <c r="H1" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="21"/>
-    </row>
-    <row r="2" spans="1:10" s="2" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I1" s="18"/>
+    </row>
+    <row r="2" spans="1:9" s="2" customFormat="1" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="13" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E2" s="13" t="s">
         <v>0</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H2" s="13" t="s">
         <v>0</v>
       </c>
       <c r="I2" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" s="22" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B3" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="7">
         <v>0.5</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="E3" s="10">
         <v>1</v>
@@ -764,7 +733,7 @@
         <v>100</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="H3" s="10">
         <v>1</v>
@@ -772,13 +741,10 @@
       <c r="I3" s="7">
         <v>10</v>
       </c>
-      <c r="J3" s="23" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B4" s="10">
         <v>31</v>
@@ -786,9 +752,6 @@
       <c r="C4" s="7">
         <v>0.3</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="E4" s="10">
         <v>28</v>
       </c>
@@ -802,7 +765,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="6"/>
       <c r="B5" s="10">
         <v>63</v>
@@ -810,8 +773,8 @@
       <c r="C5" s="7">
         <v>0.2</v>
       </c>
-      <c r="D5" s="15" t="s">
-        <v>9</v>
+      <c r="D5" s="16" t="s">
+        <v>14</v>
       </c>
       <c r="E5" s="10">
         <v>100</v>
@@ -826,7 +789,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="6"/>
       <c r="B6" s="10">
         <v>78</v>
@@ -836,8 +799,8 @@
       </c>
       <c r="E6" s="10"/>
       <c r="F6" s="7"/>
-      <c r="G6" s="15" t="s">
-        <v>8</v>
+      <c r="G6" s="16" t="s">
+        <v>13</v>
       </c>
       <c r="H6" s="10">
         <v>100</v>
@@ -846,9 +809,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
-        <v>8</v>
+    <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="16" t="s">
+        <v>13</v>
       </c>
       <c r="B7" s="10">
         <v>100</v>
@@ -861,7 +824,7 @@
       <c r="H7" s="10"/>
       <c r="I7" s="7"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="6"/>
       <c r="B8" s="10"/>
       <c r="C8" s="7"/>
@@ -870,7 +833,10 @@
       <c r="H8" s="10"/>
       <c r="I8" s="7"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="B9" s="10"/>
       <c r="C9" s="7"/>
       <c r="E9" s="10"/>
@@ -878,7 +844,10 @@
       <c r="H9" s="10"/>
       <c r="I9" s="7"/>
     </row>
-    <row r="10" spans="1:10" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="B10" s="10"/>
       <c r="C10" s="7"/>
       <c r="E10" s="10"/>
@@ -886,7 +855,10 @@
       <c r="H10" s="10"/>
       <c r="I10" s="7"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="85" x14ac:dyDescent="0.2">
+      <c r="A11" s="15" t="s">
+        <v>17</v>
+      </c>
       <c r="B11" s="10"/>
       <c r="C11" s="7"/>
       <c r="E11" s="10"/>
@@ -894,7 +866,7 @@
       <c r="H11" s="10"/>
       <c r="I11" s="7"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B12" s="10"/>
       <c r="C12" s="7"/>
       <c r="E12" s="10"/>
@@ -902,7 +874,7 @@
       <c r="H12" s="10"/>
       <c r="I12" s="7"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B13" s="10"/>
       <c r="C13" s="7"/>
       <c r="E13" s="10"/>
@@ -910,7 +882,7 @@
       <c r="H13" s="10"/>
       <c r="I13" s="7"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B14" s="10"/>
       <c r="C14" s="7"/>
       <c r="E14" s="10"/>
@@ -918,7 +890,7 @@
       <c r="H14" s="10"/>
       <c r="I14" s="7"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B15" s="10"/>
       <c r="C15" s="7"/>
       <c r="E15" s="10"/>
@@ -926,7 +898,7 @@
       <c r="H15" s="10"/>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B16" s="10"/>
       <c r="C16" s="7"/>
       <c r="E16" s="10"/>
@@ -934,7 +906,7 @@
       <c r="H16" s="10"/>
       <c r="I16" s="7"/>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B17" s="10"/>
       <c r="C17" s="7"/>
       <c r="E17" s="10"/>
@@ -942,7 +914,7 @@
       <c r="H17" s="10"/>
       <c r="I17" s="7"/>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B18" s="10"/>
       <c r="C18" s="7"/>
       <c r="E18" s="10"/>
@@ -950,7 +922,7 @@
       <c r="H18" s="10"/>
       <c r="I18" s="7"/>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B19" s="10"/>
       <c r="C19" s="7"/>
       <c r="E19" s="10"/>
@@ -958,7 +930,7 @@
       <c r="H19" s="10"/>
       <c r="I19" s="7"/>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B20" s="10"/>
       <c r="C20" s="7"/>
       <c r="E20" s="10"/>
@@ -966,7 +938,7 @@
       <c r="H20" s="10"/>
       <c r="I20" s="7"/>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B21" s="10"/>
       <c r="C21" s="7"/>
       <c r="E21" s="10"/>
@@ -974,7 +946,7 @@
       <c r="H21" s="10"/>
       <c r="I21" s="7"/>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B22" s="10"/>
       <c r="C22" s="7"/>
       <c r="E22" s="10"/>
@@ -982,7 +954,7 @@
       <c r="H22" s="10"/>
       <c r="I22" s="7"/>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B23" s="10"/>
       <c r="C23" s="7"/>
       <c r="E23" s="10"/>
@@ -990,7 +962,7 @@
       <c r="H23" s="10"/>
       <c r="I23" s="7"/>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B24" s="10"/>
       <c r="C24" s="7"/>
       <c r="E24" s="10"/>
@@ -998,7 +970,7 @@
       <c r="H24" s="10"/>
       <c r="I24" s="7"/>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B25" s="10"/>
       <c r="C25" s="7"/>
       <c r="E25" s="10"/>
@@ -1006,7 +978,7 @@
       <c r="H25" s="10"/>
       <c r="I25" s="7"/>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B26" s="10"/>
       <c r="C26" s="7"/>
       <c r="E26" s="10"/>
@@ -1014,7 +986,7 @@
       <c r="H26" s="10"/>
       <c r="I26" s="7"/>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B27" s="10"/>
       <c r="C27" s="7"/>
       <c r="E27" s="10"/>
@@ -1022,7 +994,7 @@
       <c r="H27" s="10"/>
       <c r="I27" s="7"/>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B28" s="10"/>
       <c r="C28" s="7"/>
       <c r="E28" s="10"/>
@@ -1030,7 +1002,7 @@
       <c r="H28" s="10"/>
       <c r="I28" s="7"/>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B29" s="10"/>
       <c r="C29" s="7"/>
       <c r="E29" s="10"/>
@@ -1038,7 +1010,7 @@
       <c r="H29" s="10"/>
       <c r="I29" s="7"/>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B30" s="10"/>
       <c r="C30" s="7"/>
       <c r="E30" s="10"/>
@@ -1046,7 +1018,7 @@
       <c r="H30" s="10"/>
       <c r="I30" s="7"/>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B31" s="10"/>
       <c r="C31" s="7"/>
       <c r="E31" s="10"/>
@@ -1054,7 +1026,7 @@
       <c r="H31" s="10"/>
       <c r="I31" s="7"/>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B32" s="10"/>
       <c r="C32" s="7"/>
       <c r="E32" s="10"/>
@@ -1062,7 +1034,7 @@
       <c r="H32" s="10"/>
       <c r="I32" s="7"/>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B33" s="10"/>
       <c r="C33" s="7"/>
       <c r="E33" s="10"/>
@@ -1070,7 +1042,7 @@
       <c r="H33" s="10"/>
       <c r="I33" s="7"/>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B34" s="10"/>
       <c r="C34" s="7"/>
       <c r="E34" s="10"/>
@@ -1078,7 +1050,7 @@
       <c r="H34" s="10"/>
       <c r="I34" s="7"/>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B35" s="10"/>
       <c r="C35" s="7"/>
       <c r="E35" s="10"/>
@@ -1086,7 +1058,7 @@
       <c r="H35" s="10"/>
       <c r="I35" s="7"/>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B36" s="10"/>
       <c r="C36" s="7"/>
       <c r="E36" s="10"/>
@@ -1094,7 +1066,7 @@
       <c r="H36" s="10"/>
       <c r="I36" s="7"/>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B37" s="10"/>
       <c r="C37" s="7"/>
       <c r="E37" s="10"/>
@@ -1102,7 +1074,7 @@
       <c r="H37" s="10"/>
       <c r="I37" s="7"/>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B38" s="10"/>
       <c r="C38" s="7"/>
       <c r="E38" s="10"/>
@@ -1110,7 +1082,7 @@
       <c r="H38" s="10"/>
       <c r="I38" s="7"/>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B39" s="10"/>
       <c r="C39" s="7"/>
       <c r="E39" s="10"/>
@@ -1118,7 +1090,7 @@
       <c r="H39" s="10"/>
       <c r="I39" s="7"/>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B40" s="10"/>
       <c r="C40" s="7"/>
       <c r="E40" s="10"/>
@@ -1126,7 +1098,7 @@
       <c r="H40" s="10"/>
       <c r="I40" s="7"/>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B41" s="10"/>
       <c r="C41" s="7"/>
       <c r="E41" s="10"/>
@@ -1134,7 +1106,7 @@
       <c r="H41" s="10"/>
       <c r="I41" s="7"/>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B42" s="10"/>
       <c r="C42" s="7"/>
       <c r="E42" s="10"/>
@@ -1142,7 +1114,7 @@
       <c r="H42" s="10"/>
       <c r="I42" s="7"/>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B43" s="10"/>
       <c r="C43" s="7"/>
       <c r="E43" s="10"/>
@@ -1150,7 +1122,7 @@
       <c r="H43" s="10"/>
       <c r="I43" s="7"/>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B44" s="10"/>
       <c r="C44" s="7"/>
       <c r="E44" s="10"/>
@@ -1158,7 +1130,7 @@
       <c r="H44" s="10"/>
       <c r="I44" s="7"/>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B45" s="10"/>
       <c r="C45" s="7"/>
       <c r="E45" s="10"/>
@@ -1166,7 +1138,7 @@
       <c r="H45" s="10"/>
       <c r="I45" s="7"/>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B46" s="10"/>
       <c r="C46" s="7"/>
       <c r="E46" s="10"/>
@@ -1174,7 +1146,7 @@
       <c r="H46" s="10"/>
       <c r="I46" s="7"/>
     </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B47" s="10"/>
       <c r="C47" s="7"/>
       <c r="E47" s="10"/>
@@ -1182,7 +1154,7 @@
       <c r="H47" s="10"/>
       <c r="I47" s="7"/>
     </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B48" s="10"/>
       <c r="C48" s="7"/>
       <c r="E48" s="10"/>
@@ -1190,7 +1162,7 @@
       <c r="H48" s="10"/>
       <c r="I48" s="7"/>
     </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B49" s="10"/>
       <c r="C49" s="7"/>
       <c r="E49" s="10"/>
@@ -1198,7 +1170,7 @@
       <c r="H49" s="10"/>
       <c r="I49" s="7"/>
     </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B50" s="10"/>
       <c r="C50" s="7"/>
       <c r="E50" s="10"/>
@@ -1206,7 +1178,7 @@
       <c r="H50" s="10"/>
       <c r="I50" s="7"/>
     </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B51" s="10"/>
       <c r="C51" s="7"/>
       <c r="E51" s="10"/>
@@ -1214,7 +1186,7 @@
       <c r="H51" s="10"/>
       <c r="I51" s="7"/>
     </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B52" s="10"/>
       <c r="C52" s="7"/>
       <c r="E52" s="10"/>
@@ -1222,7 +1194,7 @@
       <c r="H52" s="10"/>
       <c r="I52" s="7"/>
     </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B53" s="10"/>
       <c r="C53" s="7"/>
       <c r="E53" s="10"/>
@@ -1230,7 +1202,7 @@
       <c r="H53" s="10"/>
       <c r="I53" s="7"/>
     </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B54" s="10"/>
       <c r="C54" s="7"/>
       <c r="E54" s="10"/>
@@ -1238,7 +1210,7 @@
       <c r="H54" s="10"/>
       <c r="I54" s="7"/>
     </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B55" s="10"/>
       <c r="C55" s="7"/>
       <c r="E55" s="10"/>
@@ -1246,7 +1218,7 @@
       <c r="H55" s="10"/>
       <c r="I55" s="7"/>
     </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B56" s="10"/>
       <c r="C56" s="7"/>
       <c r="E56" s="10"/>
@@ -1254,7 +1226,7 @@
       <c r="H56" s="10"/>
       <c r="I56" s="7"/>
     </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B57" s="10"/>
       <c r="C57" s="7"/>
       <c r="E57" s="10"/>
@@ -1262,7 +1234,7 @@
       <c r="H57" s="10"/>
       <c r="I57" s="7"/>
     </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B58" s="10"/>
       <c r="C58" s="7"/>
       <c r="E58" s="10"/>
@@ -1270,7 +1242,7 @@
       <c r="H58" s="10"/>
       <c r="I58" s="7"/>
     </row>
-    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B59" s="10"/>
       <c r="C59" s="7"/>
       <c r="E59" s="10"/>
@@ -1278,7 +1250,7 @@
       <c r="H59" s="10"/>
       <c r="I59" s="7"/>
     </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B60" s="10"/>
       <c r="C60" s="7"/>
       <c r="E60" s="10"/>
@@ -1286,7 +1258,7 @@
       <c r="H60" s="10"/>
       <c r="I60" s="7"/>
     </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B61" s="10"/>
       <c r="C61" s="7"/>
       <c r="E61" s="10"/>
@@ -1294,7 +1266,7 @@
       <c r="H61" s="10"/>
       <c r="I61" s="7"/>
     </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B62" s="10"/>
       <c r="C62" s="7"/>
       <c r="E62" s="10"/>
@@ -1302,7 +1274,7 @@
       <c r="H62" s="10"/>
       <c r="I62" s="7"/>
     </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B63" s="10"/>
       <c r="C63" s="7"/>
       <c r="E63" s="10"/>
@@ -1310,7 +1282,7 @@
       <c r="H63" s="10"/>
       <c r="I63" s="7"/>
     </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B64" s="10"/>
       <c r="C64" s="7"/>
       <c r="E64" s="10"/>
@@ -1318,7 +1290,7 @@
       <c r="H64" s="10"/>
       <c r="I64" s="7"/>
     </row>
-    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B65" s="10"/>
       <c r="C65" s="7"/>
       <c r="E65" s="10"/>
@@ -1326,7 +1298,7 @@
       <c r="H65" s="10"/>
       <c r="I65" s="7"/>
     </row>
-    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B66" s="10"/>
       <c r="C66" s="7"/>
       <c r="E66" s="10"/>
@@ -1334,7 +1306,7 @@
       <c r="H66" s="10"/>
       <c r="I66" s="7"/>
     </row>
-    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B67" s="10"/>
       <c r="C67" s="7"/>
       <c r="E67" s="10"/>
@@ -1342,7 +1314,7 @@
       <c r="H67" s="10"/>
       <c r="I67" s="7"/>
     </row>
-    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B68" s="10"/>
       <c r="C68" s="7"/>
       <c r="E68" s="10"/>
@@ -1350,7 +1322,7 @@
       <c r="H68" s="10"/>
       <c r="I68" s="7"/>
     </row>
-    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B69" s="10"/>
       <c r="C69" s="7"/>
       <c r="E69" s="10"/>
@@ -1358,7 +1330,7 @@
       <c r="H69" s="10"/>
       <c r="I69" s="7"/>
     </row>
-    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B70" s="10"/>
       <c r="C70" s="7"/>
       <c r="E70" s="10"/>
@@ -1366,7 +1338,7 @@
       <c r="H70" s="10"/>
       <c r="I70" s="7"/>
     </row>
-    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B71" s="10"/>
       <c r="C71" s="7"/>
       <c r="E71" s="10"/>
@@ -1374,7 +1346,7 @@
       <c r="H71" s="10"/>
       <c r="I71" s="7"/>
     </row>
-    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B72" s="10"/>
       <c r="C72" s="7"/>
       <c r="E72" s="10"/>
@@ -1382,7 +1354,7 @@
       <c r="H72" s="10"/>
       <c r="I72" s="7"/>
     </row>
-    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B73" s="10"/>
       <c r="C73" s="7"/>
       <c r="E73" s="10"/>
@@ -1390,7 +1362,7 @@
       <c r="H73" s="10"/>
       <c r="I73" s="7"/>
     </row>
-    <row r="74" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B74" s="10"/>
       <c r="C74" s="7"/>
       <c r="E74" s="10"/>
@@ -1398,7 +1370,7 @@
       <c r="H74" s="10"/>
       <c r="I74" s="7"/>
     </row>
-    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B75" s="10"/>
       <c r="C75" s="7"/>
       <c r="E75" s="10"/>
@@ -1406,7 +1378,7 @@
       <c r="H75" s="10"/>
       <c r="I75" s="7"/>
     </row>
-    <row r="76" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B76" s="10"/>
       <c r="C76" s="7"/>
       <c r="E76" s="10"/>
@@ -1414,7 +1386,7 @@
       <c r="H76" s="10"/>
       <c r="I76" s="7"/>
     </row>
-    <row r="77" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B77" s="10"/>
       <c r="C77" s="7"/>
       <c r="E77" s="10"/>
@@ -1422,7 +1394,7 @@
       <c r="H77" s="10"/>
       <c r="I77" s="7"/>
     </row>
-    <row r="78" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B78" s="10"/>
       <c r="C78" s="7"/>
       <c r="E78" s="10"/>
@@ -1430,7 +1402,7 @@
       <c r="H78" s="10"/>
       <c r="I78" s="7"/>
     </row>
-    <row r="79" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B79" s="10"/>
       <c r="C79" s="7"/>
       <c r="E79" s="10"/>
@@ -1438,7 +1410,7 @@
       <c r="H79" s="10"/>
       <c r="I79" s="7"/>
     </row>
-    <row r="80" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B80" s="10"/>
       <c r="C80" s="7"/>
       <c r="E80" s="10"/>
@@ -1446,7 +1418,7 @@
       <c r="H80" s="10"/>
       <c r="I80" s="7"/>
     </row>
-    <row r="81" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B81" s="10"/>
       <c r="C81" s="7"/>
       <c r="E81" s="10"/>
@@ -1454,7 +1426,7 @@
       <c r="H81" s="10"/>
       <c r="I81" s="7"/>
     </row>
-    <row r="82" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B82" s="10"/>
       <c r="C82" s="7"/>
       <c r="E82" s="10"/>
@@ -1462,7 +1434,7 @@
       <c r="H82" s="10"/>
       <c r="I82" s="7"/>
     </row>
-    <row r="83" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B83" s="10"/>
       <c r="C83" s="7"/>
       <c r="E83" s="10"/>
@@ -1470,7 +1442,7 @@
       <c r="H83" s="10"/>
       <c r="I83" s="7"/>
     </row>
-    <row r="84" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B84" s="10"/>
       <c r="C84" s="7"/>
       <c r="E84" s="10"/>
@@ -1478,7 +1450,7 @@
       <c r="H84" s="10"/>
       <c r="I84" s="7"/>
     </row>
-    <row r="85" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B85" s="10"/>
       <c r="C85" s="7"/>
       <c r="E85" s="10"/>
@@ -1486,7 +1458,7 @@
       <c r="H85" s="10"/>
       <c r="I85" s="7"/>
     </row>
-    <row r="86" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B86" s="10"/>
       <c r="C86" s="7"/>
       <c r="E86" s="10"/>
@@ -1494,7 +1466,7 @@
       <c r="H86" s="10"/>
       <c r="I86" s="7"/>
     </row>
-    <row r="87" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B87" s="10"/>
       <c r="C87" s="7"/>
       <c r="E87" s="10"/>
@@ -1502,7 +1474,7 @@
       <c r="H87" s="10"/>
       <c r="I87" s="7"/>
     </row>
-    <row r="88" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B88" s="10"/>
       <c r="C88" s="7"/>
       <c r="E88" s="10"/>
@@ -1510,7 +1482,7 @@
       <c r="H88" s="10"/>
       <c r="I88" s="7"/>
     </row>
-    <row r="89" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B89" s="10"/>
       <c r="C89" s="7"/>
       <c r="E89" s="10"/>
@@ -1518,7 +1490,7 @@
       <c r="H89" s="10"/>
       <c r="I89" s="7"/>
     </row>
-    <row r="90" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B90" s="10"/>
       <c r="C90" s="7"/>
       <c r="E90" s="10"/>
@@ -1526,7 +1498,7 @@
       <c r="H90" s="10"/>
       <c r="I90" s="7"/>
     </row>
-    <row r="91" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B91" s="10"/>
       <c r="C91" s="7"/>
       <c r="E91" s="10"/>
@@ -1534,7 +1506,7 @@
       <c r="H91" s="10"/>
       <c r="I91" s="7"/>
     </row>
-    <row r="92" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B92" s="10"/>
       <c r="C92" s="7"/>
       <c r="E92" s="10"/>
@@ -1542,7 +1514,7 @@
       <c r="H92" s="10"/>
       <c r="I92" s="7"/>
     </row>
-    <row r="93" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B93" s="10"/>
       <c r="C93" s="7"/>
       <c r="E93" s="10"/>
@@ -1550,7 +1522,7 @@
       <c r="H93" s="10"/>
       <c r="I93" s="7"/>
     </row>
-    <row r="94" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B94" s="10"/>
       <c r="C94" s="7"/>
       <c r="E94" s="10"/>
@@ -1558,7 +1530,7 @@
       <c r="H94" s="10"/>
       <c r="I94" s="7"/>
     </row>
-    <row r="95" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B95" s="10"/>
       <c r="C95" s="7"/>
       <c r="E95" s="10"/>
@@ -1566,7 +1538,7 @@
       <c r="H95" s="10"/>
       <c r="I95" s="7"/>
     </row>
-    <row r="96" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B96" s="10"/>
       <c r="C96" s="7"/>
       <c r="E96" s="10"/>
@@ -1574,7 +1546,7 @@
       <c r="H96" s="10"/>
       <c r="I96" s="7"/>
     </row>
-    <row r="97" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B97" s="10"/>
       <c r="C97" s="7"/>
       <c r="E97" s="10"/>
@@ -1582,7 +1554,7 @@
       <c r="H97" s="10"/>
       <c r="I97" s="7"/>
     </row>
-    <row r="98" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B98" s="10"/>
       <c r="C98" s="7"/>
       <c r="E98" s="10"/>
@@ -1590,7 +1562,7 @@
       <c r="H98" s="10"/>
       <c r="I98" s="7"/>
     </row>
-    <row r="99" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B99" s="10"/>
       <c r="C99" s="7"/>
       <c r="E99" s="10"/>
@@ -1598,7 +1570,7 @@
       <c r="H99" s="10"/>
       <c r="I99" s="7"/>
     </row>
-    <row r="100" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B100" s="10"/>
       <c r="C100" s="7"/>
       <c r="E100" s="10"/>
@@ -1606,7 +1578,7 @@
       <c r="H100" s="10"/>
       <c r="I100" s="7"/>
     </row>
-    <row r="101" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B101" s="10"/>
       <c r="C101" s="7"/>
       <c r="E101" s="10"/>
@@ -1614,7 +1586,7 @@
       <c r="H101" s="10"/>
       <c r="I101" s="7"/>
     </row>
-    <row r="102" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B102" s="10"/>
       <c r="C102" s="7"/>
       <c r="E102" s="10"/>
@@ -1622,7 +1594,7 @@
       <c r="H102" s="10"/>
       <c r="I102" s="7"/>
     </row>
-    <row r="103" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B103" s="10"/>
       <c r="C103" s="7"/>
       <c r="E103" s="10"/>
@@ -1630,7 +1602,7 @@
       <c r="H103" s="10"/>
       <c r="I103" s="7"/>
     </row>
-    <row r="104" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B104" s="10"/>
       <c r="C104" s="7"/>
       <c r="E104" s="10"/>
@@ -1638,7 +1610,7 @@
       <c r="H104" s="10"/>
       <c r="I104" s="7"/>
     </row>
-    <row r="105" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B105" s="10"/>
       <c r="C105" s="7"/>
       <c r="E105" s="10"/>
@@ -1646,7 +1618,7 @@
       <c r="H105" s="10"/>
       <c r="I105" s="7"/>
     </row>
-    <row r="106" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B106" s="10"/>
       <c r="C106" s="7"/>
       <c r="E106" s="10"/>
@@ -1654,7 +1626,7 @@
       <c r="H106" s="10"/>
       <c r="I106" s="7"/>
     </row>
-    <row r="107" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B107" s="10"/>
       <c r="C107" s="7"/>
       <c r="E107" s="10"/>
@@ -1662,7 +1634,7 @@
       <c r="H107" s="10"/>
       <c r="I107" s="7"/>
     </row>
-    <row r="108" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B108" s="10"/>
       <c r="C108" s="7"/>
       <c r="E108" s="10"/>
@@ -1670,7 +1642,7 @@
       <c r="H108" s="10"/>
       <c r="I108" s="7"/>
     </row>
-    <row r="109" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B109" s="10"/>
       <c r="C109" s="7"/>
       <c r="E109" s="10"/>
@@ -1678,7 +1650,7 @@
       <c r="H109" s="10"/>
       <c r="I109" s="7"/>
     </row>
-    <row r="110" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B110" s="10"/>
       <c r="C110" s="7"/>
       <c r="E110" s="10"/>
@@ -1686,7 +1658,7 @@
       <c r="H110" s="10"/>
       <c r="I110" s="7"/>
     </row>
-    <row r="111" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B111" s="10"/>
       <c r="C111" s="7"/>
       <c r="E111" s="10"/>
@@ -1694,7 +1666,7 @@
       <c r="H111" s="10"/>
       <c r="I111" s="7"/>
     </row>
-    <row r="112" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B112" s="10"/>
       <c r="C112" s="7"/>
       <c r="E112" s="10"/>
@@ -1702,7 +1674,7 @@
       <c r="H112" s="10"/>
       <c r="I112" s="7"/>
     </row>
-    <row r="113" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B113" s="10"/>
       <c r="C113" s="7"/>
       <c r="E113" s="10"/>
@@ -1710,7 +1682,7 @@
       <c r="H113" s="10"/>
       <c r="I113" s="7"/>
     </row>
-    <row r="114" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B114" s="10"/>
       <c r="C114" s="7"/>
       <c r="E114" s="10"/>
@@ -1718,7 +1690,7 @@
       <c r="H114" s="10"/>
       <c r="I114" s="7"/>
     </row>
-    <row r="115" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B115" s="10"/>
       <c r="C115" s="7"/>
       <c r="E115" s="10"/>
@@ -1726,7 +1698,7 @@
       <c r="H115" s="10"/>
       <c r="I115" s="7"/>
     </row>
-    <row r="116" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B116" s="10"/>
       <c r="C116" s="7"/>
       <c r="E116" s="10"/>
@@ -1734,7 +1706,7 @@
       <c r="H116" s="10"/>
       <c r="I116" s="7"/>
     </row>
-    <row r="117" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B117" s="10"/>
       <c r="C117" s="7"/>
       <c r="E117" s="10"/>
@@ -1742,7 +1714,7 @@
       <c r="H117" s="10"/>
       <c r="I117" s="7"/>
     </row>
-    <row r="118" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B118" s="10"/>
       <c r="C118" s="7"/>
       <c r="E118" s="10"/>
@@ -1750,7 +1722,7 @@
       <c r="H118" s="10"/>
       <c r="I118" s="7"/>
     </row>
-    <row r="119" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B119" s="10"/>
       <c r="C119" s="7"/>
       <c r="E119" s="10"/>
@@ -1758,7 +1730,7 @@
       <c r="H119" s="10"/>
       <c r="I119" s="7"/>
     </row>
-    <row r="120" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B120" s="10"/>
       <c r="C120" s="7"/>
       <c r="E120" s="10"/>
@@ -1766,7 +1738,7 @@
       <c r="H120" s="10"/>
       <c r="I120" s="7"/>
     </row>
-    <row r="121" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B121" s="10"/>
       <c r="C121" s="7"/>
       <c r="E121" s="10"/>
@@ -1774,7 +1746,7 @@
       <c r="H121" s="10"/>
       <c r="I121" s="7"/>
     </row>
-    <row r="122" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B122" s="10"/>
       <c r="C122" s="7"/>
       <c r="E122" s="10"/>
@@ -1782,7 +1754,7 @@
       <c r="H122" s="10"/>
       <c r="I122" s="7"/>
     </row>
-    <row r="123" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B123" s="10"/>
       <c r="C123" s="7"/>
       <c r="E123" s="10"/>
@@ -1790,7 +1762,7 @@
       <c r="H123" s="10"/>
       <c r="I123" s="7"/>
     </row>
-    <row r="124" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B124" s="10"/>
       <c r="C124" s="7"/>
       <c r="E124" s="10"/>
@@ -1798,7 +1770,7 @@
       <c r="H124" s="10"/>
       <c r="I124" s="7"/>
     </row>
-    <row r="125" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B125" s="10"/>
       <c r="C125" s="7"/>
       <c r="E125" s="10"/>
@@ -1806,7 +1778,7 @@
       <c r="H125" s="10"/>
       <c r="I125" s="7"/>
     </row>
-    <row r="126" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B126" s="10"/>
       <c r="C126" s="7"/>
       <c r="E126" s="10"/>
@@ -1814,7 +1786,7 @@
       <c r="H126" s="10"/>
       <c r="I126" s="7"/>
     </row>
-    <row r="127" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B127" s="10"/>
       <c r="C127" s="7"/>
       <c r="E127" s="10"/>
@@ -1822,7 +1794,7 @@
       <c r="H127" s="10"/>
       <c r="I127" s="7"/>
     </row>
-    <row r="128" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B128" s="10"/>
       <c r="C128" s="7"/>
       <c r="E128" s="10"/>
@@ -1830,7 +1802,7 @@
       <c r="H128" s="10"/>
       <c r="I128" s="7"/>
     </row>
-    <row r="129" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B129" s="10"/>
       <c r="C129" s="7"/>
       <c r="E129" s="10"/>
@@ -1838,7 +1810,7 @@
       <c r="H129" s="10"/>
       <c r="I129" s="7"/>
     </row>
-    <row r="130" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B130" s="10"/>
       <c r="C130" s="7"/>
       <c r="E130" s="10"/>
@@ -1846,7 +1818,7 @@
       <c r="H130" s="10"/>
       <c r="I130" s="7"/>
     </row>
-    <row r="131" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B131" s="10"/>
       <c r="C131" s="7"/>
       <c r="E131" s="10"/>
@@ -1854,7 +1826,7 @@
       <c r="H131" s="10"/>
       <c r="I131" s="7"/>
     </row>
-    <row r="132" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B132" s="10"/>
       <c r="C132" s="7"/>
       <c r="E132" s="10"/>
@@ -1862,7 +1834,7 @@
       <c r="H132" s="10"/>
       <c r="I132" s="7"/>
     </row>
-    <row r="133" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B133" s="10"/>
       <c r="C133" s="7"/>
       <c r="E133" s="10"/>
@@ -1870,7 +1842,7 @@
       <c r="H133" s="10"/>
       <c r="I133" s="7"/>
     </row>
-    <row r="134" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B134" s="10"/>
       <c r="C134" s="7"/>
       <c r="E134" s="10"/>
@@ -1878,7 +1850,7 @@
       <c r="H134" s="10"/>
       <c r="I134" s="7"/>
     </row>
-    <row r="135" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B135" s="10"/>
       <c r="C135" s="7"/>
       <c r="E135" s="10"/>
@@ -1886,7 +1858,7 @@
       <c r="H135" s="10"/>
       <c r="I135" s="7"/>
     </row>
-    <row r="136" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B136" s="10"/>
       <c r="C136" s="7"/>
       <c r="E136" s="10"/>
@@ -1894,7 +1866,7 @@
       <c r="H136" s="10"/>
       <c r="I136" s="7"/>
     </row>
-    <row r="137" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B137" s="10"/>
       <c r="C137" s="7"/>
       <c r="E137" s="10"/>
@@ -1902,7 +1874,7 @@
       <c r="H137" s="10"/>
       <c r="I137" s="7"/>
     </row>
-    <row r="138" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B138" s="10"/>
       <c r="C138" s="7"/>
       <c r="E138" s="10"/>
@@ -1910,7 +1882,7 @@
       <c r="H138" s="10"/>
       <c r="I138" s="7"/>
     </row>
-    <row r="139" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B139" s="10"/>
       <c r="C139" s="7"/>
       <c r="E139" s="10"/>
@@ -1918,7 +1890,7 @@
       <c r="H139" s="10"/>
       <c r="I139" s="7"/>
     </row>
-    <row r="140" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B140" s="10"/>
       <c r="C140" s="7"/>
       <c r="E140" s="10"/>
@@ -1926,7 +1898,7 @@
       <c r="H140" s="10"/>
       <c r="I140" s="7"/>
     </row>
-    <row r="141" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B141" s="10"/>
       <c r="C141" s="7"/>
       <c r="E141" s="10"/>
@@ -1934,7 +1906,7 @@
       <c r="H141" s="10"/>
       <c r="I141" s="7"/>
     </row>
-    <row r="142" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B142" s="10"/>
       <c r="C142" s="7"/>
       <c r="E142" s="10"/>
@@ -1942,7 +1914,7 @@
       <c r="H142" s="10"/>
       <c r="I142" s="7"/>
     </row>
-    <row r="143" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B143" s="10"/>
       <c r="C143" s="7"/>
       <c r="E143" s="10"/>
@@ -1950,7 +1922,7 @@
       <c r="H143" s="10"/>
       <c r="I143" s="7"/>
     </row>
-    <row r="144" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B144" s="10"/>
       <c r="C144" s="7"/>
       <c r="E144" s="10"/>
@@ -1958,7 +1930,7 @@
       <c r="H144" s="10"/>
       <c r="I144" s="7"/>
     </row>
-    <row r="145" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B145" s="10"/>
       <c r="C145" s="7"/>
       <c r="E145" s="10"/>
@@ -1966,7 +1938,7 @@
       <c r="H145" s="10"/>
       <c r="I145" s="7"/>
     </row>
-    <row r="146" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B146" s="10"/>
       <c r="C146" s="7"/>
       <c r="E146" s="10"/>
@@ -1974,7 +1946,7 @@
       <c r="H146" s="10"/>
       <c r="I146" s="7"/>
     </row>
-    <row r="147" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B147" s="10"/>
       <c r="C147" s="7"/>
       <c r="E147" s="10"/>
@@ -1982,7 +1954,7 @@
       <c r="H147" s="10"/>
       <c r="I147" s="7"/>
     </row>
-    <row r="148" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B148" s="10"/>
       <c r="C148" s="7"/>
       <c r="E148" s="10"/>
@@ -1990,7 +1962,7 @@
       <c r="H148" s="10"/>
       <c r="I148" s="7"/>
     </row>
-    <row r="149" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B149" s="10"/>
       <c r="C149" s="7"/>
       <c r="E149" s="10"/>
@@ -1998,7 +1970,7 @@
       <c r="H149" s="10"/>
       <c r="I149" s="7"/>
     </row>
-    <row r="150" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B150" s="10"/>
       <c r="C150" s="7"/>
       <c r="E150" s="10"/>
@@ -2006,7 +1978,7 @@
       <c r="H150" s="10"/>
       <c r="I150" s="7"/>
     </row>
-    <row r="151" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B151" s="10"/>
       <c r="C151" s="7"/>
       <c r="E151" s="10"/>
@@ -2014,7 +1986,7 @@
       <c r="H151" s="10"/>
       <c r="I151" s="7"/>
     </row>
-    <row r="152" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B152" s="10"/>
       <c r="C152" s="7"/>
       <c r="E152" s="10"/>
@@ -2022,7 +1994,7 @@
       <c r="H152" s="10"/>
       <c r="I152" s="7"/>
     </row>
-    <row r="153" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B153" s="10"/>
       <c r="C153" s="7"/>
       <c r="E153" s="10"/>
@@ -2030,7 +2002,7 @@
       <c r="H153" s="10"/>
       <c r="I153" s="7"/>
     </row>
-    <row r="154" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B154" s="10"/>
       <c r="C154" s="7"/>
       <c r="E154" s="10"/>
@@ -2038,7 +2010,7 @@
       <c r="H154" s="10"/>
       <c r="I154" s="7"/>
     </row>
-    <row r="155" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B155" s="10"/>
       <c r="C155" s="7"/>
       <c r="E155" s="10"/>
@@ -2046,7 +2018,7 @@
       <c r="H155" s="10"/>
       <c r="I155" s="7"/>
     </row>
-    <row r="156" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B156" s="10"/>
       <c r="C156" s="7"/>
       <c r="E156" s="10"/>
@@ -2054,7 +2026,7 @@
       <c r="H156" s="10"/>
       <c r="I156" s="7"/>
     </row>
-    <row r="157" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B157" s="10"/>
       <c r="C157" s="7"/>
       <c r="E157" s="10"/>
@@ -2062,7 +2034,7 @@
       <c r="H157" s="10"/>
       <c r="I157" s="7"/>
     </row>
-    <row r="158" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B158" s="10"/>
       <c r="C158" s="7"/>
       <c r="E158" s="10"/>
@@ -2070,7 +2042,7 @@
       <c r="H158" s="10"/>
       <c r="I158" s="7"/>
     </row>
-    <row r="159" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B159" s="10"/>
       <c r="C159" s="7"/>
       <c r="E159" s="10"/>
@@ -2078,7 +2050,7 @@
       <c r="H159" s="10"/>
       <c r="I159" s="7"/>
     </row>
-    <row r="160" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B160" s="10"/>
       <c r="C160" s="7"/>
       <c r="E160" s="10"/>
@@ -2086,7 +2058,7 @@
       <c r="H160" s="10"/>
       <c r="I160" s="7"/>
     </row>
-    <row r="161" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B161" s="10"/>
       <c r="C161" s="7"/>
       <c r="E161" s="10"/>
@@ -2094,7 +2066,7 @@
       <c r="H161" s="10"/>
       <c r="I161" s="7"/>
     </row>
-    <row r="162" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="162" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B162" s="10"/>
       <c r="C162" s="7"/>
       <c r="E162" s="10"/>
@@ -2102,7 +2074,7 @@
       <c r="H162" s="10"/>
       <c r="I162" s="7"/>
     </row>
-    <row r="163" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="163" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B163" s="10"/>
       <c r="C163" s="7"/>
       <c r="E163" s="10"/>
@@ -2110,7 +2082,7 @@
       <c r="H163" s="10"/>
       <c r="I163" s="7"/>
     </row>
-    <row r="164" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="164" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B164" s="10"/>
       <c r="C164" s="7"/>
       <c r="E164" s="10"/>
@@ -2118,7 +2090,7 @@
       <c r="H164" s="10"/>
       <c r="I164" s="7"/>
     </row>
-    <row r="165" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B165" s="10"/>
       <c r="C165" s="7"/>
       <c r="E165" s="10"/>
@@ -2126,7 +2098,7 @@
       <c r="H165" s="10"/>
       <c r="I165" s="7"/>
     </row>
-    <row r="166" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B166" s="10"/>
       <c r="C166" s="7"/>
       <c r="E166" s="10"/>
@@ -2134,7 +2106,7 @@
       <c r="H166" s="10"/>
       <c r="I166" s="7"/>
     </row>
-    <row r="167" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B167" s="10"/>
       <c r="C167" s="7"/>
       <c r="E167" s="10"/>
@@ -2142,7 +2114,7 @@
       <c r="H167" s="10"/>
       <c r="I167" s="7"/>
     </row>
-    <row r="168" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="168" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B168" s="10"/>
       <c r="C168" s="7"/>
       <c r="E168" s="10"/>
@@ -2150,7 +2122,7 @@
       <c r="H168" s="10"/>
       <c r="I168" s="7"/>
     </row>
-    <row r="169" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="169" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B169" s="10"/>
       <c r="C169" s="7"/>
       <c r="E169" s="10"/>
@@ -2158,7 +2130,7 @@
       <c r="H169" s="10"/>
       <c r="I169" s="7"/>
     </row>
-    <row r="170" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="170" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B170" s="10"/>
       <c r="C170" s="7"/>
       <c r="E170" s="10"/>
@@ -2166,7 +2138,7 @@
       <c r="H170" s="10"/>
       <c r="I170" s="7"/>
     </row>
-    <row r="171" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="171" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B171" s="10"/>
       <c r="C171" s="7"/>
       <c r="E171" s="10"/>
@@ -2174,7 +2146,7 @@
       <c r="H171" s="10"/>
       <c r="I171" s="7"/>
     </row>
-    <row r="172" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="172" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B172" s="10"/>
       <c r="C172" s="7"/>
       <c r="E172" s="10"/>
@@ -2182,7 +2154,7 @@
       <c r="H172" s="10"/>
       <c r="I172" s="7"/>
     </row>
-    <row r="173" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="173" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B173" s="10"/>
       <c r="C173" s="7"/>
       <c r="E173" s="10"/>
@@ -2190,7 +2162,7 @@
       <c r="H173" s="10"/>
       <c r="I173" s="7"/>
     </row>
-    <row r="174" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="174" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B174" s="10"/>
       <c r="C174" s="7"/>
       <c r="E174" s="10"/>
@@ -2198,7 +2170,7 @@
       <c r="H174" s="10"/>
       <c r="I174" s="7"/>
     </row>
-    <row r="175" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="175" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B175" s="10"/>
       <c r="C175" s="7"/>
       <c r="E175" s="10"/>
@@ -2206,7 +2178,7 @@
       <c r="H175" s="10"/>
       <c r="I175" s="7"/>
     </row>
-    <row r="176" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="176" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B176" s="10"/>
       <c r="C176" s="7"/>
       <c r="E176" s="10"/>
@@ -2214,7 +2186,7 @@
       <c r="H176" s="10"/>
       <c r="I176" s="7"/>
     </row>
-    <row r="177" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B177" s="10"/>
       <c r="C177" s="7"/>
       <c r="E177" s="10"/>
@@ -2222,7 +2194,7 @@
       <c r="H177" s="10"/>
       <c r="I177" s="7"/>
     </row>
-    <row r="178" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B178" s="10"/>
       <c r="C178" s="7"/>
       <c r="E178" s="10"/>
@@ -2230,7 +2202,7 @@
       <c r="H178" s="10"/>
       <c r="I178" s="7"/>
     </row>
-    <row r="179" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B179" s="10"/>
       <c r="C179" s="7"/>
       <c r="E179" s="10"/>
@@ -2238,7 +2210,7 @@
       <c r="H179" s="10"/>
       <c r="I179" s="7"/>
     </row>
-    <row r="180" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="180" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B180" s="10"/>
       <c r="C180" s="7"/>
       <c r="E180" s="10"/>
@@ -2246,7 +2218,7 @@
       <c r="H180" s="10"/>
       <c r="I180" s="7"/>
     </row>
-    <row r="181" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="181" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B181" s="10"/>
       <c r="C181" s="7"/>
       <c r="E181" s="10"/>
@@ -2254,7 +2226,7 @@
       <c r="H181" s="10"/>
       <c r="I181" s="7"/>
     </row>
-    <row r="182" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="182" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B182" s="10"/>
       <c r="C182" s="7"/>
       <c r="E182" s="10"/>
@@ -2262,7 +2234,7 @@
       <c r="H182" s="10"/>
       <c r="I182" s="7"/>
     </row>
-    <row r="183" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="183" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B183" s="10"/>
       <c r="C183" s="7"/>
       <c r="E183" s="10"/>
@@ -2270,7 +2242,7 @@
       <c r="H183" s="10"/>
       <c r="I183" s="7"/>
     </row>
-    <row r="184" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="184" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B184" s="10"/>
       <c r="C184" s="7"/>
       <c r="E184" s="10"/>
@@ -2278,7 +2250,7 @@
       <c r="H184" s="10"/>
       <c r="I184" s="7"/>
     </row>
-    <row r="185" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="185" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B185" s="10"/>
       <c r="C185" s="7"/>
       <c r="E185" s="10"/>
@@ -2286,7 +2258,7 @@
       <c r="H185" s="10"/>
       <c r="I185" s="7"/>
     </row>
-    <row r="186" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="186" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B186" s="10"/>
       <c r="C186" s="7"/>
       <c r="E186" s="10"/>
@@ -2294,7 +2266,7 @@
       <c r="H186" s="10"/>
       <c r="I186" s="7"/>
     </row>
-    <row r="187" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="187" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B187" s="10"/>
       <c r="C187" s="7"/>
       <c r="E187" s="10"/>
@@ -2302,7 +2274,7 @@
       <c r="H187" s="10"/>
       <c r="I187" s="7"/>
     </row>
-    <row r="188" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="188" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B188" s="10"/>
       <c r="C188" s="7"/>
       <c r="E188" s="10"/>
@@ -2310,7 +2282,7 @@
       <c r="H188" s="10"/>
       <c r="I188" s="7"/>
     </row>
-    <row r="189" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="189" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B189" s="10"/>
       <c r="C189" s="7"/>
       <c r="E189" s="10"/>
@@ -2318,7 +2290,7 @@
       <c r="H189" s="10"/>
       <c r="I189" s="7"/>
     </row>
-    <row r="190" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="190" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B190" s="10"/>
       <c r="C190" s="7"/>
       <c r="E190" s="10"/>
@@ -2326,7 +2298,7 @@
       <c r="H190" s="10"/>
       <c r="I190" s="7"/>
     </row>
-    <row r="191" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="191" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B191" s="10"/>
       <c r="C191" s="7"/>
       <c r="E191" s="10"/>
@@ -2334,7 +2306,7 @@
       <c r="H191" s="10"/>
       <c r="I191" s="7"/>
     </row>
-    <row r="192" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="192" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B192" s="10"/>
       <c r="C192" s="7"/>
       <c r="E192" s="10"/>
@@ -2342,7 +2314,7 @@
       <c r="H192" s="10"/>
       <c r="I192" s="7"/>
     </row>
-    <row r="193" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="193" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B193" s="10"/>
       <c r="C193" s="7"/>
       <c r="E193" s="10"/>
@@ -2350,7 +2322,7 @@
       <c r="H193" s="10"/>
       <c r="I193" s="7"/>
     </row>
-    <row r="194" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="194" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B194" s="10"/>
       <c r="C194" s="7"/>
       <c r="E194" s="10"/>
@@ -2358,7 +2330,7 @@
       <c r="H194" s="10"/>
       <c r="I194" s="7"/>
     </row>
-    <row r="195" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="195" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B195" s="10"/>
       <c r="C195" s="7"/>
       <c r="E195" s="10"/>
@@ -2366,7 +2338,7 @@
       <c r="H195" s="10"/>
       <c r="I195" s="7"/>
     </row>
-    <row r="196" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="196" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B196" s="10"/>
       <c r="C196" s="7"/>
       <c r="E196" s="10"/>
@@ -2374,7 +2346,7 @@
       <c r="H196" s="10"/>
       <c r="I196" s="7"/>
     </row>
-    <row r="197" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="197" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B197" s="10"/>
       <c r="C197" s="7"/>
       <c r="E197" s="10"/>
@@ -2382,7 +2354,7 @@
       <c r="H197" s="10"/>
       <c r="I197" s="7"/>
     </row>
-    <row r="198" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="198" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B198" s="10"/>
       <c r="C198" s="7"/>
       <c r="E198" s="10"/>
@@ -2390,7 +2362,7 @@
       <c r="H198" s="10"/>
       <c r="I198" s="7"/>
     </row>
-    <row r="199" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="199" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B199" s="10"/>
       <c r="C199" s="7"/>
       <c r="E199" s="10"/>
@@ -2398,7 +2370,7 @@
       <c r="H199" s="10"/>
       <c r="I199" s="7"/>
     </row>
-    <row r="200" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="200" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B200" s="10"/>
       <c r="C200" s="7"/>
       <c r="E200" s="10"/>
@@ -2406,7 +2378,7 @@
       <c r="H200" s="10"/>
       <c r="I200" s="7"/>
     </row>
-    <row r="201" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="201" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B201" s="10"/>
       <c r="C201" s="7"/>
       <c r="E201" s="10"/>
@@ -2414,7 +2386,7 @@
       <c r="H201" s="10"/>
       <c r="I201" s="7"/>
     </row>
-    <row r="202" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="202" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B202" s="10"/>
       <c r="C202" s="7"/>
       <c r="E202" s="10"/>
@@ -2422,7 +2394,7 @@
       <c r="H202" s="10"/>
       <c r="I202" s="7"/>
     </row>
-    <row r="203" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="203" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B203" s="10"/>
       <c r="C203" s="7"/>
       <c r="E203" s="10"/>
@@ -2430,7 +2402,7 @@
       <c r="H203" s="10"/>
       <c r="I203" s="7"/>
     </row>
-    <row r="204" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="204" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B204" s="10"/>
       <c r="C204" s="7"/>
       <c r="E204" s="10"/>
@@ -2438,7 +2410,7 @@
       <c r="H204" s="10"/>
       <c r="I204" s="7"/>
     </row>
-    <row r="205" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="205" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B205" s="10"/>
       <c r="C205" s="7"/>
       <c r="E205" s="10"/>
@@ -2446,7 +2418,7 @@
       <c r="H205" s="10"/>
       <c r="I205" s="7"/>
     </row>
-    <row r="206" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="206" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B206" s="10"/>
       <c r="C206" s="7"/>
       <c r="E206" s="10"/>
@@ -2454,7 +2426,7 @@
       <c r="H206" s="10"/>
       <c r="I206" s="7"/>
     </row>
-    <row r="207" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="207" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B207" s="10"/>
       <c r="C207" s="7"/>
       <c r="E207" s="10"/>
@@ -2462,7 +2434,7 @@
       <c r="H207" s="10"/>
       <c r="I207" s="7"/>
     </row>
-    <row r="208" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="208" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B208" s="10"/>
       <c r="C208" s="7"/>
       <c r="E208" s="10"/>
@@ -2470,7 +2442,7 @@
       <c r="H208" s="10"/>
       <c r="I208" s="7"/>
     </row>
-    <row r="209" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="209" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B209" s="10"/>
       <c r="C209" s="7"/>
       <c r="E209" s="10"/>
@@ -2478,7 +2450,7 @@
       <c r="H209" s="10"/>
       <c r="I209" s="7"/>
     </row>
-    <row r="210" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="210" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B210" s="10"/>
       <c r="C210" s="7"/>
       <c r="E210" s="10"/>
@@ -2486,7 +2458,7 @@
       <c r="H210" s="10"/>
       <c r="I210" s="7"/>
     </row>
-    <row r="211" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="211" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B211" s="10"/>
       <c r="C211" s="7"/>
       <c r="E211" s="10"/>
@@ -2494,7 +2466,7 @@
       <c r="H211" s="10"/>
       <c r="I211" s="7"/>
     </row>
-    <row r="212" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="212" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B212" s="10"/>
       <c r="C212" s="7"/>
       <c r="E212" s="10"/>
@@ -2502,7 +2474,7 @@
       <c r="H212" s="10"/>
       <c r="I212" s="7"/>
     </row>
-    <row r="213" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="213" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B213" s="10"/>
       <c r="C213" s="7"/>
       <c r="E213" s="10"/>
@@ -2510,7 +2482,7 @@
       <c r="H213" s="10"/>
       <c r="I213" s="7"/>
     </row>
-    <row r="214" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="214" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B214" s="10"/>
       <c r="C214" s="7"/>
       <c r="E214" s="10"/>
@@ -2518,7 +2490,7 @@
       <c r="H214" s="10"/>
       <c r="I214" s="7"/>
     </row>
-    <row r="215" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="215" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B215" s="10"/>
       <c r="C215" s="7"/>
       <c r="E215" s="10"/>
@@ -2526,7 +2498,7 @@
       <c r="H215" s="10"/>
       <c r="I215" s="7"/>
     </row>
-    <row r="216" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="216" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B216" s="10"/>
       <c r="C216" s="7"/>
       <c r="E216" s="10"/>
@@ -2534,7 +2506,7 @@
       <c r="H216" s="10"/>
       <c r="I216" s="7"/>
     </row>
-    <row r="217" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="217" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B217" s="10"/>
       <c r="C217" s="7"/>
       <c r="E217" s="10"/>
@@ -2542,7 +2514,7 @@
       <c r="H217" s="10"/>
       <c r="I217" s="7"/>
     </row>
-    <row r="218" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="218" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B218" s="10"/>
       <c r="C218" s="7"/>
       <c r="E218" s="10"/>
@@ -2550,7 +2522,7 @@
       <c r="H218" s="10"/>
       <c r="I218" s="7"/>
     </row>
-    <row r="219" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="219" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B219" s="10"/>
       <c r="C219" s="7"/>
       <c r="E219" s="10"/>
@@ -2558,7 +2530,7 @@
       <c r="H219" s="10"/>
       <c r="I219" s="7"/>
     </row>
-    <row r="220" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="220" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B220" s="10"/>
       <c r="C220" s="7"/>
       <c r="E220" s="10"/>
@@ -2566,7 +2538,7 @@
       <c r="H220" s="10"/>
       <c r="I220" s="7"/>
     </row>
-    <row r="221" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="221" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B221" s="10"/>
       <c r="C221" s="7"/>
       <c r="E221" s="10"/>
@@ -2574,7 +2546,7 @@
       <c r="H221" s="10"/>
       <c r="I221" s="7"/>
     </row>
-    <row r="222" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="222" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B222" s="10"/>
       <c r="C222" s="7"/>
       <c r="E222" s="10"/>
@@ -2582,7 +2554,7 @@
       <c r="H222" s="10"/>
       <c r="I222" s="7"/>
     </row>
-    <row r="223" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="223" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B223" s="10"/>
       <c r="C223" s="7"/>
       <c r="E223" s="10"/>
@@ -2590,7 +2562,7 @@
       <c r="H223" s="10"/>
       <c r="I223" s="7"/>
     </row>
-    <row r="224" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="224" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B224" s="10"/>
       <c r="C224" s="7"/>
       <c r="E224" s="10"/>
@@ -2598,7 +2570,7 @@
       <c r="H224" s="10"/>
       <c r="I224" s="7"/>
     </row>
-    <row r="225" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="225" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B225" s="10"/>
       <c r="C225" s="7"/>
       <c r="E225" s="10"/>
@@ -2606,7 +2578,7 @@
       <c r="H225" s="10"/>
       <c r="I225" s="7"/>
     </row>
-    <row r="226" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="226" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B226" s="10"/>
       <c r="C226" s="7"/>
       <c r="E226" s="10"/>
@@ -2614,7 +2586,7 @@
       <c r="H226" s="10"/>
       <c r="I226" s="7"/>
     </row>
-    <row r="227" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="227" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B227" s="10"/>
       <c r="C227" s="7"/>
       <c r="E227" s="10"/>
@@ -2622,7 +2594,7 @@
       <c r="H227" s="10"/>
       <c r="I227" s="7"/>
     </row>
-    <row r="228" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="228" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B228" s="10"/>
       <c r="C228" s="7"/>
       <c r="E228" s="10"/>
@@ -2630,7 +2602,7 @@
       <c r="H228" s="10"/>
       <c r="I228" s="7"/>
     </row>
-    <row r="229" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="229" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B229" s="10"/>
       <c r="C229" s="7"/>
       <c r="E229" s="10"/>
@@ -2638,7 +2610,7 @@
       <c r="H229" s="10"/>
       <c r="I229" s="7"/>
     </row>
-    <row r="230" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="230" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B230" s="10"/>
       <c r="C230" s="7"/>
       <c r="E230" s="10"/>
@@ -2646,7 +2618,7 @@
       <c r="H230" s="10"/>
       <c r="I230" s="7"/>
     </row>
-    <row r="231" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="231" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B231" s="10"/>
       <c r="C231" s="7"/>
       <c r="E231" s="10"/>
@@ -2654,7 +2626,7 @@
       <c r="H231" s="10"/>
       <c r="I231" s="7"/>
     </row>
-    <row r="232" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="232" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B232" s="10"/>
       <c r="C232" s="7"/>
       <c r="E232" s="10"/>
@@ -2662,7 +2634,7 @@
       <c r="H232" s="10"/>
       <c r="I232" s="7"/>
     </row>
-    <row r="233" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="233" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B233" s="10"/>
       <c r="C233" s="7"/>
       <c r="E233" s="10"/>
@@ -2670,7 +2642,7 @@
       <c r="H233" s="10"/>
       <c r="I233" s="7"/>
     </row>
-    <row r="234" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="234" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B234" s="10"/>
       <c r="C234" s="7"/>
       <c r="E234" s="10"/>
@@ -2678,7 +2650,7 @@
       <c r="H234" s="10"/>
       <c r="I234" s="7"/>
     </row>
-    <row r="235" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="235" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B235" s="10"/>
       <c r="C235" s="7"/>
       <c r="E235" s="10"/>
@@ -2686,7 +2658,7 @@
       <c r="H235" s="10"/>
       <c r="I235" s="7"/>
     </row>
-    <row r="236" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="236" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B236" s="10"/>
       <c r="C236" s="7"/>
       <c r="E236" s="10"/>
@@ -2694,7 +2666,7 @@
       <c r="H236" s="10"/>
       <c r="I236" s="7"/>
     </row>
-    <row r="237" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="237" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B237" s="10"/>
       <c r="C237" s="7"/>
       <c r="E237" s="10"/>
@@ -2702,7 +2674,7 @@
       <c r="H237" s="10"/>
       <c r="I237" s="7"/>
     </row>
-    <row r="238" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="238" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B238" s="10"/>
       <c r="C238" s="7"/>
       <c r="E238" s="10"/>
@@ -2710,7 +2682,7 @@
       <c r="H238" s="10"/>
       <c r="I238" s="7"/>
     </row>
-    <row r="239" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="239" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B239" s="10"/>
       <c r="C239" s="7"/>
       <c r="E239" s="10"/>
@@ -2718,7 +2690,7 @@
       <c r="H239" s="10"/>
       <c r="I239" s="7"/>
     </row>
-    <row r="240" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="240" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B240" s="10"/>
       <c r="C240" s="7"/>
       <c r="E240" s="10"/>
@@ -2726,7 +2698,7 @@
       <c r="H240" s="10"/>
       <c r="I240" s="7"/>
     </row>
-    <row r="241" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="241" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B241" s="10"/>
       <c r="C241" s="7"/>
       <c r="E241" s="10"/>
@@ -2734,7 +2706,7 @@
       <c r="H241" s="10"/>
       <c r="I241" s="7"/>
     </row>
-    <row r="242" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="242" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B242" s="10"/>
       <c r="C242" s="7"/>
       <c r="E242" s="10"/>
@@ -2742,7 +2714,7 @@
       <c r="H242" s="10"/>
       <c r="I242" s="7"/>
     </row>
-    <row r="243" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="243" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B243" s="10"/>
       <c r="C243" s="7"/>
       <c r="E243" s="10"/>
@@ -2750,7 +2722,7 @@
       <c r="H243" s="10"/>
       <c r="I243" s="7"/>
     </row>
-    <row r="244" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="244" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B244" s="10"/>
       <c r="C244" s="7"/>
       <c r="E244" s="10"/>
@@ -2758,7 +2730,7 @@
       <c r="H244" s="10"/>
       <c r="I244" s="7"/>
     </row>
-    <row r="245" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="245" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B245" s="10"/>
       <c r="C245" s="7"/>
       <c r="E245" s="10"/>
@@ -2766,7 +2738,7 @@
       <c r="H245" s="10"/>
       <c r="I245" s="7"/>
     </row>
-    <row r="246" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="246" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B246" s="10"/>
       <c r="C246" s="7"/>
       <c r="E246" s="10"/>
@@ -2774,7 +2746,7 @@
       <c r="H246" s="10"/>
       <c r="I246" s="7"/>
     </row>
-    <row r="247" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="247" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B247" s="10"/>
       <c r="C247" s="7"/>
       <c r="E247" s="10"/>
@@ -2782,7 +2754,7 @@
       <c r="H247" s="10"/>
       <c r="I247" s="7"/>
     </row>
-    <row r="248" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="248" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B248" s="10"/>
       <c r="C248" s="7"/>
       <c r="E248" s="10"/>
@@ -2790,7 +2762,7 @@
       <c r="H248" s="10"/>
       <c r="I248" s="7"/>
     </row>
-    <row r="249" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="249" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B249" s="10"/>
       <c r="C249" s="7"/>
       <c r="E249" s="10"/>
@@ -2798,7 +2770,7 @@
       <c r="H249" s="10"/>
       <c r="I249" s="7"/>
     </row>
-    <row r="250" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="250" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B250" s="10"/>
       <c r="C250" s="7"/>
       <c r="E250" s="10"/>
@@ -2806,7 +2778,7 @@
       <c r="H250" s="10"/>
       <c r="I250" s="7"/>
     </row>
-    <row r="251" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="251" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B251" s="10"/>
       <c r="C251" s="7"/>
       <c r="E251" s="10"/>
@@ -2814,7 +2786,7 @@
       <c r="H251" s="10"/>
       <c r="I251" s="7"/>
     </row>
-    <row r="252" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="252" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B252" s="10"/>
       <c r="C252" s="7"/>
       <c r="E252" s="10"/>
@@ -2822,7 +2794,7 @@
       <c r="H252" s="10"/>
       <c r="I252" s="7"/>
     </row>
-    <row r="253" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="253" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B253" s="10"/>
       <c r="C253" s="7"/>
       <c r="E253" s="10"/>
@@ -2830,7 +2802,7 @@
       <c r="H253" s="10"/>
       <c r="I253" s="7"/>
     </row>
-    <row r="254" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="254" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B254" s="10"/>
       <c r="C254" s="7"/>
       <c r="E254" s="10"/>
@@ -2838,7 +2810,7 @@
       <c r="H254" s="10"/>
       <c r="I254" s="7"/>
     </row>
-    <row r="255" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="255" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B255" s="10"/>
       <c r="C255" s="7"/>
       <c r="E255" s="10"/>
@@ -2846,7 +2818,7 @@
       <c r="H255" s="10"/>
       <c r="I255" s="7"/>
     </row>
-    <row r="256" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="256" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B256" s="10"/>
       <c r="C256" s="7"/>
       <c r="E256" s="10"/>
@@ -2854,7 +2826,7 @@
       <c r="H256" s="10"/>
       <c r="I256" s="7"/>
     </row>
-    <row r="257" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="257" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B257" s="10"/>
       <c r="C257" s="7"/>
       <c r="E257" s="10"/>
@@ -2862,7 +2834,7 @@
       <c r="H257" s="10"/>
       <c r="I257" s="7"/>
     </row>
-    <row r="258" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="258" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B258" s="10"/>
       <c r="C258" s="7"/>
       <c r="E258" s="10"/>
@@ -2870,7 +2842,7 @@
       <c r="H258" s="10"/>
       <c r="I258" s="7"/>
     </row>
-    <row r="259" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="259" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B259" s="10"/>
       <c r="C259" s="7"/>
       <c r="E259" s="10"/>
@@ -2878,7 +2850,7 @@
       <c r="H259" s="10"/>
       <c r="I259" s="7"/>
     </row>
-    <row r="260" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="260" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B260" s="10"/>
       <c r="C260" s="7"/>
       <c r="E260" s="10"/>
@@ -2886,7 +2858,7 @@
       <c r="H260" s="10"/>
       <c r="I260" s="7"/>
     </row>
-    <row r="261" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="261" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B261" s="10"/>
       <c r="C261" s="7"/>
       <c r="E261" s="10"/>
@@ -2894,7 +2866,7 @@
       <c r="H261" s="10"/>
       <c r="I261" s="7"/>
     </row>
-    <row r="262" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="262" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B262" s="10"/>
       <c r="C262" s="7"/>
       <c r="E262" s="10"/>
@@ -2902,7 +2874,7 @@
       <c r="H262" s="10"/>
       <c r="I262" s="7"/>
     </row>
-    <row r="263" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="263" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B263" s="10"/>
       <c r="C263" s="7"/>
       <c r="E263" s="10"/>
@@ -2910,7 +2882,7 @@
       <c r="H263" s="10"/>
       <c r="I263" s="7"/>
     </row>
-    <row r="264" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="264" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B264" s="10"/>
       <c r="C264" s="7"/>
       <c r="E264" s="10"/>
@@ -2918,7 +2890,7 @@
       <c r="H264" s="10"/>
       <c r="I264" s="7"/>
     </row>
-    <row r="265" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="265" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B265" s="10"/>
       <c r="C265" s="7"/>
       <c r="E265" s="10"/>
@@ -2926,7 +2898,7 @@
       <c r="H265" s="10"/>
       <c r="I265" s="7"/>
     </row>
-    <row r="266" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="266" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B266" s="10"/>
       <c r="C266" s="7"/>
       <c r="E266" s="10"/>
@@ -2934,7 +2906,7 @@
       <c r="H266" s="10"/>
       <c r="I266" s="7"/>
     </row>
-    <row r="267" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="267" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B267" s="10"/>
       <c r="C267" s="7"/>
       <c r="E267" s="10"/>
@@ -2942,7 +2914,7 @@
       <c r="H267" s="10"/>
       <c r="I267" s="7"/>
     </row>
-    <row r="268" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="268" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B268" s="10"/>
       <c r="C268" s="7"/>
       <c r="E268" s="10"/>
@@ -2950,7 +2922,7 @@
       <c r="H268" s="10"/>
       <c r="I268" s="7"/>
     </row>
-    <row r="269" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="269" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B269" s="10"/>
       <c r="C269" s="7"/>
       <c r="E269" s="10"/>
@@ -2958,7 +2930,7 @@
       <c r="H269" s="10"/>
       <c r="I269" s="7"/>
     </row>
-    <row r="270" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="270" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B270" s="10"/>
       <c r="C270" s="7"/>
       <c r="E270" s="10"/>
@@ -2966,7 +2938,7 @@
       <c r="H270" s="10"/>
       <c r="I270" s="7"/>
     </row>
-    <row r="271" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="271" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B271" s="10"/>
       <c r="C271" s="7"/>
       <c r="E271" s="10"/>
@@ -2974,7 +2946,7 @@
       <c r="H271" s="10"/>
       <c r="I271" s="7"/>
     </row>
-    <row r="272" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="272" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B272" s="10"/>
       <c r="C272" s="7"/>
       <c r="E272" s="10"/>
@@ -2982,7 +2954,7 @@
       <c r="H272" s="10"/>
       <c r="I272" s="7"/>
     </row>
-    <row r="273" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="273" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B273" s="10"/>
       <c r="C273" s="7"/>
       <c r="E273" s="10"/>
@@ -2990,7 +2962,7 @@
       <c r="H273" s="10"/>
       <c r="I273" s="7"/>
     </row>
-    <row r="274" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="274" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B274" s="10"/>
       <c r="C274" s="7"/>
       <c r="E274" s="10"/>
@@ -2998,7 +2970,7 @@
       <c r="H274" s="10"/>
       <c r="I274" s="7"/>
     </row>
-    <row r="275" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="275" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B275" s="10"/>
       <c r="C275" s="7"/>
       <c r="E275" s="10"/>
@@ -3006,7 +2978,7 @@
       <c r="H275" s="10"/>
       <c r="I275" s="7"/>
     </row>
-    <row r="276" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="276" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B276" s="10"/>
       <c r="C276" s="7"/>
       <c r="E276" s="10"/>
@@ -3014,7 +2986,7 @@
       <c r="H276" s="10"/>
       <c r="I276" s="7"/>
     </row>
-    <row r="277" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="277" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B277" s="10"/>
       <c r="C277" s="7"/>
       <c r="E277" s="10"/>
@@ -3022,7 +2994,7 @@
       <c r="H277" s="10"/>
       <c r="I277" s="7"/>
     </row>
-    <row r="278" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="278" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B278" s="10"/>
       <c r="C278" s="7"/>
       <c r="E278" s="10"/>
@@ -3030,7 +3002,7 @@
       <c r="H278" s="10"/>
       <c r="I278" s="7"/>
     </row>
-    <row r="279" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="279" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B279" s="10"/>
       <c r="C279" s="7"/>
       <c r="E279" s="10"/>
@@ -3038,7 +3010,7 @@
       <c r="H279" s="10"/>
       <c r="I279" s="7"/>
     </row>
-    <row r="280" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="280" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B280" s="10"/>
       <c r="C280" s="7"/>
       <c r="E280" s="10"/>
@@ -3046,7 +3018,7 @@
       <c r="H280" s="10"/>
       <c r="I280" s="7"/>
     </row>
-    <row r="281" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="281" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B281" s="10"/>
       <c r="C281" s="7"/>
       <c r="E281" s="10"/>
@@ -3054,7 +3026,7 @@
       <c r="H281" s="10"/>
       <c r="I281" s="7"/>
     </row>
-    <row r="282" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="282" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B282" s="10"/>
       <c r="C282" s="7"/>
       <c r="E282" s="10"/>
@@ -3062,7 +3034,7 @@
       <c r="H282" s="10"/>
       <c r="I282" s="7"/>
     </row>
-    <row r="283" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="283" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B283" s="10"/>
       <c r="C283" s="7"/>
       <c r="E283" s="10"/>
@@ -3070,7 +3042,7 @@
       <c r="H283" s="10"/>
       <c r="I283" s="7"/>
     </row>
-    <row r="284" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="284" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B284" s="10"/>
       <c r="C284" s="7"/>
       <c r="E284" s="10"/>
@@ -3078,7 +3050,7 @@
       <c r="H284" s="10"/>
       <c r="I284" s="7"/>
     </row>
-    <row r="285" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="285" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B285" s="10"/>
       <c r="C285" s="7"/>
       <c r="E285" s="10"/>
@@ -3086,7 +3058,7 @@
       <c r="H285" s="10"/>
       <c r="I285" s="7"/>
     </row>
-    <row r="286" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="286" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B286" s="10"/>
       <c r="C286" s="7"/>
       <c r="E286" s="10"/>
@@ -3094,7 +3066,7 @@
       <c r="H286" s="10"/>
       <c r="I286" s="7"/>
     </row>
-    <row r="287" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="287" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B287" s="10"/>
       <c r="C287" s="7"/>
       <c r="E287" s="10"/>
@@ -3102,7 +3074,7 @@
       <c r="H287" s="10"/>
       <c r="I287" s="7"/>
     </row>
-    <row r="288" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="288" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B288" s="10"/>
       <c r="C288" s="7"/>
       <c r="E288" s="10"/>
@@ -3110,7 +3082,7 @@
       <c r="H288" s="10"/>
       <c r="I288" s="7"/>
     </row>
-    <row r="289" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="289" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B289" s="10"/>
       <c r="C289" s="7"/>
       <c r="E289" s="10"/>
@@ -3118,7 +3090,7 @@
       <c r="H289" s="10"/>
       <c r="I289" s="7"/>
     </row>
-    <row r="290" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="290" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B290" s="10"/>
       <c r="C290" s="7"/>
       <c r="E290" s="10"/>
@@ -3126,7 +3098,7 @@
       <c r="H290" s="10"/>
       <c r="I290" s="7"/>
     </row>
-    <row r="291" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="291" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B291" s="10"/>
       <c r="C291" s="7"/>
       <c r="E291" s="10"/>
@@ -3134,7 +3106,7 @@
       <c r="H291" s="10"/>
       <c r="I291" s="7"/>
     </row>
-    <row r="292" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="292" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B292" s="10"/>
       <c r="C292" s="7"/>
       <c r="E292" s="10"/>
@@ -3142,7 +3114,7 @@
       <c r="H292" s="10"/>
       <c r="I292" s="7"/>
     </row>
-    <row r="293" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="293" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B293" s="10"/>
       <c r="C293" s="7"/>
       <c r="E293" s="10"/>
@@ -3150,7 +3122,7 @@
       <c r="H293" s="10"/>
       <c r="I293" s="7"/>
     </row>
-    <row r="294" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="294" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B294" s="10"/>
       <c r="C294" s="7"/>
       <c r="E294" s="10"/>
@@ -3158,7 +3130,7 @@
       <c r="H294" s="10"/>
       <c r="I294" s="7"/>
     </row>
-    <row r="295" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="295" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B295" s="10"/>
       <c r="C295" s="7"/>
       <c r="E295" s="10"/>
@@ -3166,7 +3138,7 @@
       <c r="H295" s="10"/>
       <c r="I295" s="7"/>
     </row>
-    <row r="296" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="296" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B296" s="10"/>
       <c r="C296" s="7"/>
       <c r="E296" s="10"/>
@@ -3174,7 +3146,7 @@
       <c r="H296" s="10"/>
       <c r="I296" s="7"/>
     </row>
-    <row r="297" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="297" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B297" s="10"/>
       <c r="C297" s="7"/>
       <c r="E297" s="10"/>
@@ -3182,7 +3154,7 @@
       <c r="H297" s="10"/>
       <c r="I297" s="7"/>
     </row>
-    <row r="298" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="298" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B298" s="10"/>
       <c r="C298" s="7"/>
       <c r="E298" s="10"/>
@@ -3190,7 +3162,7 @@
       <c r="H298" s="10"/>
       <c r="I298" s="7"/>
     </row>
-    <row r="299" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="299" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B299" s="10"/>
       <c r="C299" s="7"/>
       <c r="E299" s="10"/>
@@ -3198,7 +3170,7 @@
       <c r="H299" s="10"/>
       <c r="I299" s="7"/>
     </row>
-    <row r="300" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="300" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B300" s="10"/>
       <c r="C300" s="7"/>
       <c r="E300" s="10"/>
@@ -3206,7 +3178,7 @@
       <c r="H300" s="10"/>
       <c r="I300" s="7"/>
     </row>
-    <row r="301" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="301" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B301" s="10"/>
       <c r="C301" s="7"/>
       <c r="E301" s="10"/>
@@ -3214,7 +3186,7 @@
       <c r="H301" s="10"/>
       <c r="I301" s="7"/>
     </row>
-    <row r="302" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="302" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B302" s="10"/>
       <c r="C302" s="7"/>
       <c r="E302" s="10"/>
@@ -3222,7 +3194,7 @@
       <c r="H302" s="10"/>
       <c r="I302" s="7"/>
     </row>
-    <row r="303" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="303" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B303" s="10"/>
       <c r="C303" s="7"/>
       <c r="E303" s="10"/>
@@ -3230,7 +3202,7 @@
       <c r="H303" s="10"/>
       <c r="I303" s="7"/>
     </row>
-    <row r="304" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="304" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B304" s="10"/>
       <c r="C304" s="7"/>
       <c r="E304" s="10"/>
@@ -3238,7 +3210,7 @@
       <c r="H304" s="10"/>
       <c r="I304" s="7"/>
     </row>
-    <row r="305" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="305" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B305" s="10"/>
       <c r="C305" s="7"/>
       <c r="E305" s="10"/>
@@ -3246,7 +3218,7 @@
       <c r="H305" s="10"/>
       <c r="I305" s="7"/>
     </row>
-    <row r="306" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="306" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B306" s="10"/>
       <c r="C306" s="7"/>
       <c r="E306" s="10"/>
@@ -3254,7 +3226,7 @@
       <c r="H306" s="10"/>
       <c r="I306" s="7"/>
     </row>
-    <row r="307" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="307" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B307" s="10"/>
       <c r="C307" s="7"/>
       <c r="E307" s="10"/>
@@ -3262,7 +3234,7 @@
       <c r="H307" s="10"/>
       <c r="I307" s="7"/>
     </row>
-    <row r="308" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="308" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B308" s="10"/>
       <c r="C308" s="7"/>
       <c r="E308" s="10"/>
@@ -3270,7 +3242,7 @@
       <c r="H308" s="10"/>
       <c r="I308" s="7"/>
     </row>
-    <row r="309" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="309" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B309" s="10"/>
       <c r="C309" s="7"/>
       <c r="E309" s="10"/>
@@ -3278,7 +3250,7 @@
       <c r="H309" s="10"/>
       <c r="I309" s="7"/>
     </row>
-    <row r="310" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="310" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B310" s="10"/>
       <c r="C310" s="7"/>
       <c r="E310" s="10"/>
@@ -3286,7 +3258,7 @@
       <c r="H310" s="10"/>
       <c r="I310" s="7"/>
     </row>
-    <row r="311" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="311" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B311" s="10"/>
       <c r="C311" s="7"/>
       <c r="E311" s="10"/>
@@ -3294,7 +3266,7 @@
       <c r="H311" s="10"/>
       <c r="I311" s="7"/>
     </row>
-    <row r="312" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="312" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B312" s="10"/>
       <c r="C312" s="7"/>
       <c r="E312" s="10"/>
@@ -3302,7 +3274,7 @@
       <c r="H312" s="10"/>
       <c r="I312" s="7"/>
     </row>
-    <row r="313" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="313" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B313" s="10"/>
       <c r="C313" s="7"/>
       <c r="E313" s="10"/>
@@ -3310,7 +3282,7 @@
       <c r="H313" s="10"/>
       <c r="I313" s="7"/>
     </row>
-    <row r="314" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="314" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B314" s="10"/>
       <c r="C314" s="7"/>
       <c r="E314" s="10"/>
@@ -3318,7 +3290,7 @@
       <c r="H314" s="10"/>
       <c r="I314" s="7"/>
     </row>
-    <row r="315" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="315" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B315" s="10"/>
       <c r="C315" s="7"/>
       <c r="E315" s="10"/>
@@ -3326,7 +3298,7 @@
       <c r="H315" s="10"/>
       <c r="I315" s="7"/>
     </row>
-    <row r="316" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="316" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B316" s="10"/>
       <c r="C316" s="7"/>
       <c r="E316" s="10"/>
@@ -3334,7 +3306,7 @@
       <c r="H316" s="10"/>
       <c r="I316" s="7"/>
     </row>
-    <row r="317" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="317" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B317" s="10"/>
       <c r="C317" s="7"/>
       <c r="E317" s="10"/>
@@ -3342,7 +3314,7 @@
       <c r="H317" s="10"/>
       <c r="I317" s="7"/>
     </row>
-    <row r="318" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="318" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B318" s="10"/>
       <c r="C318" s="7"/>
       <c r="E318" s="10"/>
@@ -3350,7 +3322,7 @@
       <c r="H318" s="10"/>
       <c r="I318" s="7"/>
     </row>
-    <row r="319" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="319" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B319" s="10"/>
       <c r="C319" s="7"/>
       <c r="E319" s="10"/>
@@ -3358,7 +3330,7 @@
       <c r="H319" s="10"/>
       <c r="I319" s="7"/>
     </row>
-    <row r="320" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="320" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B320" s="10"/>
       <c r="C320" s="7"/>
       <c r="E320" s="10"/>
@@ -3366,7 +3338,7 @@
       <c r="H320" s="10"/>
       <c r="I320" s="7"/>
     </row>
-    <row r="321" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="321" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B321" s="10"/>
       <c r="C321" s="7"/>
       <c r="E321" s="10"/>
@@ -3374,7 +3346,7 @@
       <c r="H321" s="10"/>
       <c r="I321" s="7"/>
     </row>
-    <row r="322" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="322" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B322" s="10"/>
       <c r="C322" s="7"/>
       <c r="E322" s="10"/>
@@ -3382,7 +3354,7 @@
       <c r="H322" s="10"/>
       <c r="I322" s="7"/>
     </row>
-    <row r="323" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="323" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B323" s="10"/>
       <c r="C323" s="7"/>
       <c r="E323" s="10"/>
@@ -3390,7 +3362,7 @@
       <c r="H323" s="10"/>
       <c r="I323" s="7"/>
     </row>
-    <row r="324" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="324" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B324" s="10"/>
       <c r="C324" s="7"/>
       <c r="E324" s="10"/>
@@ -3398,7 +3370,7 @@
       <c r="H324" s="10"/>
       <c r="I324" s="7"/>
     </row>
-    <row r="325" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="325" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B325" s="10"/>
       <c r="C325" s="7"/>
       <c r="E325" s="10"/>
@@ -3406,7 +3378,7 @@
       <c r="H325" s="10"/>
       <c r="I325" s="7"/>
     </row>
-    <row r="326" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="326" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B326" s="10"/>
       <c r="C326" s="7"/>
       <c r="E326" s="10"/>
@@ -3414,7 +3386,7 @@
       <c r="H326" s="10"/>
       <c r="I326" s="7"/>
     </row>
-    <row r="327" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="327" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B327" s="10"/>
       <c r="C327" s="7"/>
       <c r="E327" s="10"/>
@@ -3422,7 +3394,7 @@
       <c r="H327" s="10"/>
       <c r="I327" s="7"/>
     </row>
-    <row r="328" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="328" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B328" s="10"/>
       <c r="C328" s="7"/>
       <c r="E328" s="10"/>
@@ -3430,7 +3402,7 @@
       <c r="H328" s="10"/>
       <c r="I328" s="7"/>
     </row>
-    <row r="329" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="329" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B329" s="10"/>
       <c r="C329" s="7"/>
       <c r="E329" s="10"/>
@@ -3438,7 +3410,7 @@
       <c r="H329" s="10"/>
       <c r="I329" s="7"/>
     </row>
-    <row r="330" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="330" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B330" s="10"/>
       <c r="C330" s="7"/>
       <c r="E330" s="10"/>
@@ -3446,7 +3418,7 @@
       <c r="H330" s="10"/>
       <c r="I330" s="7"/>
     </row>
-    <row r="331" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="331" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B331" s="10"/>
       <c r="C331" s="7"/>
       <c r="E331" s="10"/>
@@ -3454,7 +3426,7 @@
       <c r="H331" s="10"/>
       <c r="I331" s="7"/>
     </row>
-    <row r="332" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="332" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B332" s="10"/>
       <c r="C332" s="7"/>
       <c r="E332" s="10"/>
@@ -3462,7 +3434,7 @@
       <c r="H332" s="10"/>
       <c r="I332" s="7"/>
     </row>
-    <row r="333" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="333" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B333" s="10"/>
       <c r="C333" s="7"/>
       <c r="E333" s="10"/>
@@ -3470,7 +3442,7 @@
       <c r="H333" s="10"/>
       <c r="I333" s="7"/>
     </row>
-    <row r="334" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="334" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B334" s="10"/>
       <c r="C334" s="7"/>
       <c r="E334" s="10"/>
@@ -3478,7 +3450,7 @@
       <c r="H334" s="10"/>
       <c r="I334" s="7"/>
     </row>
-    <row r="335" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="335" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B335" s="10"/>
       <c r="C335" s="7"/>
       <c r="E335" s="10"/>
@@ -3486,7 +3458,7 @@
       <c r="H335" s="10"/>
       <c r="I335" s="7"/>
     </row>
-    <row r="336" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="336" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B336" s="10"/>
       <c r="C336" s="7"/>
       <c r="E336" s="10"/>
@@ -3494,7 +3466,7 @@
       <c r="H336" s="10"/>
       <c r="I336" s="7"/>
     </row>
-    <row r="337" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="337" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B337" s="10"/>
       <c r="C337" s="7"/>
       <c r="E337" s="10"/>
@@ -3502,7 +3474,7 @@
       <c r="H337" s="10"/>
       <c r="I337" s="7"/>
     </row>
-    <row r="338" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="338" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B338" s="10"/>
       <c r="C338" s="7"/>
       <c r="E338" s="10"/>
@@ -3510,7 +3482,7 @@
       <c r="H338" s="10"/>
       <c r="I338" s="7"/>
     </row>
-    <row r="339" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="339" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B339" s="10"/>
       <c r="C339" s="7"/>
       <c r="E339" s="10"/>
@@ -3518,7 +3490,7 @@
       <c r="H339" s="10"/>
       <c r="I339" s="7"/>
     </row>
-    <row r="340" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="340" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B340" s="10"/>
       <c r="C340" s="7"/>
       <c r="E340" s="10"/>
@@ -3526,7 +3498,7 @@
       <c r="H340" s="10"/>
       <c r="I340" s="7"/>
     </row>
-    <row r="341" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="341" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B341" s="10"/>
       <c r="C341" s="7"/>
       <c r="E341" s="10"/>
@@ -3534,7 +3506,7 @@
       <c r="H341" s="10"/>
       <c r="I341" s="7"/>
     </row>
-    <row r="342" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="342" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B342" s="10"/>
       <c r="C342" s="7"/>
       <c r="E342" s="10"/>
@@ -3542,7 +3514,7 @@
       <c r="H342" s="10"/>
       <c r="I342" s="7"/>
     </row>
-    <row r="343" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="343" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B343" s="10"/>
       <c r="C343" s="7"/>
       <c r="E343" s="10"/>
@@ -3550,7 +3522,7 @@
       <c r="H343" s="10"/>
       <c r="I343" s="7"/>
     </row>
-    <row r="344" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="344" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B344" s="10"/>
       <c r="C344" s="7"/>
       <c r="E344" s="10"/>
@@ -3558,7 +3530,7 @@
       <c r="H344" s="10"/>
       <c r="I344" s="7"/>
     </row>
-    <row r="345" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="345" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B345" s="10"/>
       <c r="C345" s="7"/>
       <c r="E345" s="10"/>
@@ -3566,7 +3538,7 @@
       <c r="H345" s="10"/>
       <c r="I345" s="7"/>
     </row>
-    <row r="346" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="346" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B346" s="10"/>
       <c r="C346" s="7"/>
       <c r="E346" s="10"/>
@@ -3574,7 +3546,7 @@
       <c r="H346" s="10"/>
       <c r="I346" s="7"/>
     </row>
-    <row r="347" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="347" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B347" s="10"/>
       <c r="C347" s="7"/>
       <c r="E347" s="10"/>
@@ -3582,7 +3554,7 @@
       <c r="H347" s="10"/>
       <c r="I347" s="7"/>
     </row>
-    <row r="348" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="348" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B348" s="10"/>
       <c r="C348" s="7"/>
       <c r="E348" s="10"/>
@@ -3590,7 +3562,7 @@
       <c r="H348" s="10"/>
       <c r="I348" s="7"/>
     </row>
-    <row r="349" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="349" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B349" s="10"/>
       <c r="C349" s="7"/>
       <c r="E349" s="10"/>
@@ -3598,7 +3570,7 @@
       <c r="H349" s="10"/>
       <c r="I349" s="7"/>
     </row>
-    <row r="350" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="350" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B350" s="10"/>
       <c r="C350" s="7"/>
       <c r="E350" s="10"/>
@@ -3606,7 +3578,7 @@
       <c r="H350" s="10"/>
       <c r="I350" s="7"/>
     </row>
-    <row r="351" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="351" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B351" s="10"/>
       <c r="C351" s="7"/>
       <c r="E351" s="10"/>
@@ -3614,7 +3586,7 @@
       <c r="H351" s="10"/>
       <c r="I351" s="7"/>
     </row>
-    <row r="352" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="352" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B352" s="10"/>
       <c r="C352" s="7"/>
       <c r="E352" s="10"/>
@@ -3622,7 +3594,7 @@
       <c r="H352" s="10"/>
       <c r="I352" s="7"/>
     </row>
-    <row r="353" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="353" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B353" s="10"/>
       <c r="C353" s="7"/>
       <c r="E353" s="10"/>
@@ -3630,7 +3602,7 @@
       <c r="H353" s="10"/>
       <c r="I353" s="7"/>
     </row>
-    <row r="354" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="354" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B354" s="10"/>
       <c r="C354" s="7"/>
       <c r="E354" s="10"/>
@@ -3638,7 +3610,7 @@
       <c r="H354" s="10"/>
       <c r="I354" s="7"/>
     </row>
-    <row r="355" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="355" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B355" s="10"/>
       <c r="C355" s="7"/>
       <c r="E355" s="10"/>
@@ -3646,7 +3618,7 @@
       <c r="H355" s="10"/>
       <c r="I355" s="7"/>
     </row>
-    <row r="356" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="356" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B356" s="10"/>
       <c r="C356" s="7"/>
       <c r="E356" s="10"/>
@@ -3654,7 +3626,7 @@
       <c r="H356" s="10"/>
       <c r="I356" s="7"/>
     </row>
-    <row r="357" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="357" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B357" s="10"/>
       <c r="C357" s="7"/>
       <c r="E357" s="10"/>
@@ -3662,7 +3634,7 @@
       <c r="H357" s="10"/>
       <c r="I357" s="7"/>
     </row>
-    <row r="358" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="358" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B358" s="10"/>
       <c r="C358" s="7"/>
       <c r="E358" s="10"/>
@@ -3670,7 +3642,7 @@
       <c r="H358" s="10"/>
       <c r="I358" s="7"/>
     </row>
-    <row r="359" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="359" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B359" s="10"/>
       <c r="C359" s="7"/>
       <c r="E359" s="10"/>
@@ -3678,7 +3650,7 @@
       <c r="H359" s="10"/>
       <c r="I359" s="7"/>
     </row>
-    <row r="360" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="360" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B360" s="10"/>
       <c r="C360" s="7"/>
       <c r="E360" s="10"/>
@@ -3686,7 +3658,7 @@
       <c r="H360" s="10"/>
       <c r="I360" s="7"/>
     </row>
-    <row r="361" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="361" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B361" s="10"/>
       <c r="C361" s="7"/>
       <c r="E361" s="10"/>
@@ -3694,7 +3666,7 @@
       <c r="H361" s="10"/>
       <c r="I361" s="7"/>
     </row>
-    <row r="362" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="362" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B362" s="10"/>
       <c r="C362" s="7"/>
       <c r="E362" s="10"/>
@@ -3702,7 +3674,7 @@
       <c r="H362" s="10"/>
       <c r="I362" s="7"/>
     </row>
-    <row r="363" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="363" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B363" s="10"/>
       <c r="C363" s="7"/>
       <c r="E363" s="10"/>
@@ -3710,7 +3682,7 @@
       <c r="H363" s="10"/>
       <c r="I363" s="7"/>
     </row>
-    <row r="364" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="364" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B364" s="10"/>
       <c r="C364" s="7"/>
       <c r="E364" s="10"/>
@@ -3718,7 +3690,7 @@
       <c r="H364" s="10"/>
       <c r="I364" s="7"/>
     </row>
-    <row r="365" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="365" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B365" s="10"/>
       <c r="C365" s="7"/>
       <c r="E365" s="10"/>
@@ -3726,7 +3698,7 @@
       <c r="H365" s="10"/>
       <c r="I365" s="7"/>
     </row>
-    <row r="366" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="366" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B366" s="10"/>
       <c r="C366" s="7"/>
       <c r="E366" s="10"/>
@@ -3734,7 +3706,7 @@
       <c r="H366" s="10"/>
       <c r="I366" s="7"/>
     </row>
-    <row r="367" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="367" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B367" s="10"/>
       <c r="C367" s="7"/>
       <c r="E367" s="10"/>
@@ -3742,7 +3714,7 @@
       <c r="H367" s="10"/>
       <c r="I367" s="7"/>
     </row>
-    <row r="368" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="368" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B368" s="10"/>
       <c r="C368" s="7"/>
       <c r="E368" s="10"/>
@@ -3750,7 +3722,7 @@
       <c r="H368" s="10"/>
       <c r="I368" s="7"/>
     </row>
-    <row r="369" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="369" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B369" s="10"/>
       <c r="C369" s="7"/>
       <c r="E369" s="10"/>
@@ -3758,7 +3730,7 @@
       <c r="H369" s="10"/>
       <c r="I369" s="7"/>
     </row>
-    <row r="370" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="370" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B370" s="10"/>
       <c r="C370" s="7"/>
       <c r="E370" s="10"/>
@@ -3766,7 +3738,7 @@
       <c r="H370" s="10"/>
       <c r="I370" s="7"/>
     </row>
-    <row r="371" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="371" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B371" s="10"/>
       <c r="C371" s="7"/>
       <c r="E371" s="10"/>
@@ -3774,7 +3746,7 @@
       <c r="H371" s="10"/>
       <c r="I371" s="7"/>
     </row>
-    <row r="372" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="372" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B372" s="10"/>
       <c r="C372" s="7"/>
       <c r="E372" s="10"/>
@@ -3782,7 +3754,7 @@
       <c r="H372" s="10"/>
       <c r="I372" s="7"/>
     </row>
-    <row r="373" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="373" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B373" s="10"/>
       <c r="C373" s="7"/>
       <c r="E373" s="10"/>
@@ -3790,7 +3762,7 @@
       <c r="H373" s="10"/>
       <c r="I373" s="7"/>
     </row>
-    <row r="374" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="374" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B374" s="10"/>
       <c r="C374" s="7"/>
       <c r="E374" s="10"/>
@@ -3798,7 +3770,7 @@
       <c r="H374" s="10"/>
       <c r="I374" s="7"/>
     </row>
-    <row r="375" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="375" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B375" s="10"/>
       <c r="C375" s="7"/>
       <c r="E375" s="10"/>
@@ -3806,7 +3778,7 @@
       <c r="H375" s="10"/>
       <c r="I375" s="7"/>
     </row>
-    <row r="376" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="376" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B376" s="10"/>
       <c r="C376" s="7"/>
       <c r="E376" s="10"/>
@@ -3814,7 +3786,7 @@
       <c r="H376" s="10"/>
       <c r="I376" s="7"/>
     </row>
-    <row r="377" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="377" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B377" s="10"/>
       <c r="C377" s="7"/>
       <c r="E377" s="10"/>
@@ -3822,7 +3794,7 @@
       <c r="H377" s="10"/>
       <c r="I377" s="7"/>
     </row>
-    <row r="378" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="378" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B378" s="10"/>
       <c r="C378" s="7"/>
       <c r="E378" s="10"/>
@@ -3830,7 +3802,7 @@
       <c r="H378" s="10"/>
       <c r="I378" s="7"/>
     </row>
-    <row r="379" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="379" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B379" s="10"/>
       <c r="C379" s="7"/>
       <c r="E379" s="10"/>
@@ -3838,7 +3810,7 @@
       <c r="H379" s="10"/>
       <c r="I379" s="7"/>
     </row>
-    <row r="380" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="380" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B380" s="10"/>
       <c r="C380" s="7"/>
       <c r="E380" s="10"/>
@@ -3846,7 +3818,7 @@
       <c r="H380" s="10"/>
       <c r="I380" s="7"/>
     </row>
-    <row r="381" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="381" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B381" s="10"/>
       <c r="C381" s="7"/>
       <c r="E381" s="10"/>
@@ -3854,7 +3826,7 @@
       <c r="H381" s="10"/>
       <c r="I381" s="7"/>
     </row>
-    <row r="382" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="382" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B382" s="10"/>
       <c r="C382" s="7"/>
       <c r="E382" s="10"/>
@@ -3862,7 +3834,7 @@
       <c r="H382" s="10"/>
       <c r="I382" s="7"/>
     </row>
-    <row r="383" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="383" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B383" s="10"/>
       <c r="C383" s="7"/>
       <c r="E383" s="10"/>
@@ -3870,7 +3842,7 @@
       <c r="H383" s="10"/>
       <c r="I383" s="7"/>
     </row>
-    <row r="384" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="384" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B384" s="10"/>
       <c r="C384" s="7"/>
       <c r="E384" s="10"/>
@@ -3878,7 +3850,7 @@
       <c r="H384" s="10"/>
       <c r="I384" s="7"/>
     </row>
-    <row r="385" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="385" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B385" s="10"/>
       <c r="C385" s="7"/>
       <c r="E385" s="10"/>
@@ -3886,7 +3858,7 @@
       <c r="H385" s="10"/>
       <c r="I385" s="7"/>
     </row>
-    <row r="386" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="386" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B386" s="10"/>
       <c r="C386" s="7"/>
       <c r="E386" s="10"/>
@@ -3894,7 +3866,7 @@
       <c r="H386" s="10"/>
       <c r="I386" s="7"/>
     </row>
-    <row r="387" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="387" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B387" s="10"/>
       <c r="C387" s="7"/>
       <c r="E387" s="10"/>
@@ -3902,7 +3874,7 @@
       <c r="H387" s="10"/>
       <c r="I387" s="7"/>
     </row>
-    <row r="388" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="388" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B388" s="10"/>
       <c r="C388" s="7"/>
       <c r="E388" s="10"/>
@@ -3910,7 +3882,7 @@
       <c r="H388" s="10"/>
       <c r="I388" s="7"/>
     </row>
-    <row r="389" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="389" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B389" s="10"/>
       <c r="C389" s="7"/>
       <c r="E389" s="10"/>
@@ -3918,7 +3890,7 @@
       <c r="H389" s="10"/>
       <c r="I389" s="7"/>
     </row>
-    <row r="390" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="390" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B390" s="11"/>
       <c r="C390" s="8"/>
       <c r="E390" s="11"/>
@@ -3938,65 +3910,54 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="57.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="57.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>15</v>
       </c>
       <c r="B2">
         <v>43.61</v>
       </c>
-      <c r="C2" s="18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>43.61</v>
       </c>
-      <c r="C3" s="19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="16">
-        <v>105.8</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
     </row>
   </sheetData>

</xml_diff>